<commit_message>
Added GEMx Calibration Puck Code
</commit_message>
<xml_diff>
--- a/Data/NASA_EMIT_Campaign_062024/Level1/Codes.xlsx
+++ b/Data/NASA_EMIT_Campaign_062024/Level1/Codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wksmith/Mountain Studies Dropbox/William Smith/Mac/Documents/GitHub/NASA_EMIT_Biocrust/Data/NASA_EMIT_Campaign_062024/Level1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wksmith/Documents/GitHub/NASA_EMIT_Biocrust/Data/NASA_EMIT_Campaign_062024/Level1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A781484-75A9-2548-BD57-65699D1E53A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758B98D4-AD3D-D140-B691-1604CF4D9C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14020" yWindow="-24920" windowWidth="35840" windowHeight="20600" xr2:uid="{251BB9F0-C71F-4356-9F6C-93F1D214ED6F}"/>
+    <workbookView xWindow="4480" yWindow="-25760" windowWidth="35840" windowHeight="20600" xr2:uid="{251BB9F0-C71F-4356-9F6C-93F1D214ED6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>full name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>ARSP</t>
   </si>
@@ -183,12 +177,6 @@
     <t>Indian ricegrass</t>
   </si>
   <si>
-    <t>Common name</t>
-  </si>
-  <si>
-    <t>Biocrust</t>
-  </si>
-  <si>
     <t>DCY</t>
   </si>
   <si>
@@ -213,9 +201,6 @@
     <t>SQUA</t>
   </si>
   <si>
-    <t>Squamulose Lichen</t>
-  </si>
-  <si>
     <t>BGR</t>
   </si>
   <si>
@@ -238,16 +223,70 @@
   </si>
   <si>
     <t>Pinus edulis</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Common Name</t>
+  </si>
+  <si>
+    <t>Scientific Name</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>Sand Flats</t>
+  </si>
+  <si>
+    <t>Indian Creek 1</t>
+  </si>
+  <si>
+    <t>Indian Creek 3</t>
+  </si>
+  <si>
+    <t>Indian Creek 2</t>
+  </si>
+  <si>
+    <t>Site Code</t>
+  </si>
+  <si>
+    <t>Vascular Code</t>
+  </si>
+  <si>
+    <t>Biocrust Code</t>
+  </si>
+  <si>
+    <t>Collema tenax (Lichen)</t>
+  </si>
+  <si>
+    <t>Squamulose (Lichen)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -589,283 +628,328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{741830D2-0C36-4F33-8401-893669C5DBBB}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
         <v>58</v>
       </c>
-      <c r="B25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>